<commit_message>
Chore: changed col names in excel file + improved input validation
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -486,14 +486,14 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="75.8542510121458"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.5910931174089"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -532,7 +532,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,20 +617,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2672064777328"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7246963562753"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,14 +641,8 @@
       <c r="C1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
@@ -660,14 +652,8 @@
       <c r="C2" s="0" t="n">
         <v>1.10350536706976</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>-22.0149320730417</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>1.10350536706976</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
@@ -677,14 +663,8 @@
       <c r="C3" s="0" t="n">
         <v>2.12397436954052E-007</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>0.285369137837419</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
@@ -694,14 +674,8 @@
       <c r="C4" s="0" t="n">
         <v>3.18755368558865E-009</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.0578197638950879</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
@@ -711,14 +685,8 @@
       <c r="C5" s="0" t="n">
         <v>3.33787220043099E-011</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>-0.00439408376660814</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -728,14 +696,8 @@
       <c r="C6" s="0" t="n">
         <v>2.00430304742416E-005</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>6.84865633256387</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
@@ -743,12 +705,6 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>-0.00242684925806694</v>
-      </c>
-      <c r="E7" s="0" t="n">
         <v>6.60284204552005E-011</v>
       </c>
     </row>
@@ -776,9 +732,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.9676113360324"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9878542510121"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1017,7 +973,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7327935222672"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1333,17 +1289,17 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -2672,9 +2628,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9028340080972"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9959514170041"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7611336032389"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3123,9 +3079,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0890688259109"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3117408906883"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3738,9 +3694,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2186234817814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Docs: changed flux units in toy_model to mmol/L/h
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="103">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -244,10 +244,7 @@
     <t>max (M)</t>
   </si>
   <si>
-    <t>vref_mean (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t>vref_std (umol/gCDW/h)</t>
+    <t>vref_std (mmol/L/h)</t>
   </si>
   <si>
     <t>reaction/enzyme ID</t>
@@ -486,14 +483,14 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="76.5910931174089"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -619,15 +616,15 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6072874493927"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9716599190283"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -639,7 +636,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,24 +729,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +970,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -982,13 +979,13 @@
         <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,11 +1292,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.7408906882591"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -1309,37 +1306,37 @@
         <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,13 +1344,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>23</v>
@@ -1370,16 +1367,16 @@
         <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1393,16 +1390,16 @@
         <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1419,13 +1416,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1439,13 +1436,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1459,16 +1456,16 @@
         <v>43</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1482,16 +1479,16 @@
         <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>26</v>
@@ -1508,7 +1505,7 @@
         <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1522,7 +1519,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1536,7 +1533,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1550,7 +1547,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1564,7 +1561,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1578,7 +1575,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1592,7 +1589,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -2628,9 +2625,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3079,9 +3076,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3694,9 +3691,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Chore: updating io toy_model files
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,313 +34,313 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="103">
   <si>
-    <t>General Reaction and Sampling Platform (GRASP)</t>
-  </si>
-  <si>
-    <t>Model name</t>
-  </si>
-  <si>
-    <t>toy_model</t>
-  </si>
-  <si>
-    <t>Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>ORACLE</t>
-  </si>
-  <si>
-    <t>NLP solver (NLOPT, OPTI, FMINCON (default))</t>
-  </si>
-  <si>
-    <t>FMINCON</t>
-  </si>
-  <si>
-    <t>Number of exp. conditions (excluding reference state)</t>
-  </si>
-  <si>
-    <t>Number of model structures</t>
-  </si>
-  <si>
-    <t>Number of models</t>
-  </si>
-  <si>
-    <t>Parallel mode (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t>Percentile of alive models for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Compute thermodynamics (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Initial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t>Final tolerance (in the case of ORACLE, set to 1)</t>
-  </si>
-  <si>
-    <t>rxn ID</t>
-  </si>
-  <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>m4</t>
-  </si>
-  <si>
-    <t>m5</t>
-  </si>
-  <si>
-    <t>m6</t>
-  </si>
-  <si>
-    <t>m7</t>
-  </si>
-  <si>
-    <t>m8</t>
-  </si>
-  <si>
-    <t>m9</t>
-  </si>
-  <si>
-    <t>m10</t>
-  </si>
-  <si>
-    <t>m11</t>
-  </si>
-  <si>
-    <t>m12</t>
-  </si>
-  <si>
-    <t>m13</t>
-  </si>
-  <si>
-    <t>m14</t>
-  </si>
-  <si>
-    <t>m15</t>
-  </si>
-  <si>
-    <t>m16</t>
-  </si>
-  <si>
-    <t>m17</t>
-  </si>
-  <si>
-    <t>m18</t>
-  </si>
-  <si>
-    <t>m19</t>
-  </si>
-  <si>
-    <t>m20</t>
-  </si>
-  <si>
-    <t>r1</t>
-  </si>
-  <si>
-    <t>r2</t>
-  </si>
-  <si>
-    <t>r3</t>
-  </si>
-  <si>
-    <t>r4_1</t>
-  </si>
-  <si>
-    <t>r4_2</t>
-  </si>
-  <si>
-    <t>r5</t>
-  </si>
-  <si>
-    <t>r6</t>
-  </si>
-  <si>
-    <t>r7</t>
-  </si>
-  <si>
-    <t>r8</t>
-  </si>
-  <si>
-    <t>r9</t>
-  </si>
-  <si>
-    <t>r10</t>
-  </si>
-  <si>
-    <t>r11</t>
-  </si>
-  <si>
-    <t>r12</t>
-  </si>
-  <si>
-    <t>r13</t>
-  </si>
-  <si>
-    <t>metabolite ID</t>
-  </si>
-  <si>
-    <t>Metabolite name</t>
-  </si>
-  <si>
-    <t>balanced?</t>
-  </si>
-  <si>
-    <t>active?</t>
-  </si>
-  <si>
-    <t>constant?</t>
-  </si>
-  <si>
-    <t>measured?</t>
-  </si>
-  <si>
-    <t>reaction ID</t>
-  </si>
-  <si>
-    <t>reaction name</t>
-  </si>
-  <si>
-    <t>transport reaction?</t>
-  </si>
-  <si>
-    <t>modelled?</t>
-  </si>
-  <si>
-    <t>isoenzymes</t>
-  </si>
-  <si>
-    <t>r4 1</t>
-  </si>
-  <si>
-    <t>r4</t>
-  </si>
-  <si>
-    <t>r4 2</t>
-  </si>
-  <si>
-    <t>∆Gr'_min (kJ/mol)</t>
-  </si>
-  <si>
-    <t>∆Gr'_max (kJ/mol)</t>
-  </si>
-  <si>
-    <t>min (M)</t>
-  </si>
-  <si>
-    <t>max (M)</t>
-  </si>
-  <si>
-    <t>vref_std (mmol/L/h)</t>
-  </si>
-  <si>
-    <t>reaction/enzyme ID</t>
-  </si>
-  <si>
-    <t>lower_bound</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>upper_bound</t>
-  </si>
-  <si>
-    <t>kinetic mechanism</t>
-  </si>
-  <si>
-    <t>substrate order</t>
-  </si>
-  <si>
-    <t>product order</t>
-  </si>
-  <si>
-    <t>promiscuous</t>
-  </si>
-  <si>
-    <t>inhibitors</t>
-  </si>
-  <si>
-    <t>activators</t>
-  </si>
-  <si>
-    <t>negative effector</t>
-  </si>
-  <si>
-    <t>positive effector</t>
-  </si>
-  <si>
-    <t>allosteric</t>
-  </si>
-  <si>
-    <t>subunits</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>substrateInhibOrderedBiBi</t>
-  </si>
-  <si>
-    <t>m3 m6</t>
-  </si>
-  <si>
-    <t>m5 m14</t>
-  </si>
-  <si>
-    <t>UniUniPromiscuous</t>
-  </si>
-  <si>
-    <t>m5 m6</t>
-  </si>
-  <si>
-    <t>m7 m10</t>
-  </si>
-  <si>
-    <t>r2 r5</t>
-  </si>
-  <si>
-    <t>OrdPromiscCompInhibIndep</t>
-  </si>
-  <si>
-    <t>m1 m7 m1 m10</t>
-  </si>
-  <si>
-    <t>m8 m11 m12 m12</t>
-  </si>
-  <si>
-    <t>r3 r6</t>
-  </si>
-  <si>
-    <t>orderedBiBi</t>
-  </si>
-  <si>
-    <t>m2 m8 </t>
-  </si>
-  <si>
-    <t>m9 m13</t>
-  </si>
-  <si>
-    <t>massAction</t>
-  </si>
-  <si>
-    <t>diffusion</t>
-  </si>
-  <si>
-    <t>fixedExchange</t>
+    <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toy_model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORACLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP solver (NLOPT, OPTI, FMINCON (default))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMINCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of model structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel mode (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentile of alive models for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute thermodynamics (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial tolerance (OPTIONAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final tolerance (in the case of ORACLE, set to 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolite ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolite name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balanced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constant?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measured?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport reaction?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelled?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isoenzymes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r4 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_min (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_max (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_std (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction/enzyme ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower_bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper_bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinetic mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrate order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inhibitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative effector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive effector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allosteric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subunits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrateInhibOrderedBiBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3 m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5 m14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniUniPromiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m5 m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m7 m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2 r5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OrdPromiscCompInhibIndep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m1 m7 m1 m10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m8 m11 m12 m12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r3 r6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderedBiBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2 m8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m9 m13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">massAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diffusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixedExchange</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -483,15 +483,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="G4:G7 B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,7 +601,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -616,16 +616,16 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="G4:G7 C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6072874493927"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9716599190283"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +708,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -723,16 +723,16 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="G4:G7 C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,7 +948,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -963,15 +963,15 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="G4:G7 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,7 +1271,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1286,19 +1286,19 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3481781376518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1601,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1616,13 +1616,13 @@
   </sheetPr>
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="G4:G7 D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2603,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2618,17 +2618,17 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4:G7 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3054,7 +3054,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3069,17 +3069,17 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="G4:G7 E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3304,7 +3304,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3319,13 +3319,13 @@
   </sheetPr>
   <dimension ref="A2:A16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="G4:G7 F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,7 +3406,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3421,13 +3421,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="1" sqref="G4:G7 G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3538,7 +3538,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3553,13 +3553,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="G4:G7 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,7 +3670,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3685,16 +3685,16 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="G4:G7 C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,7 +3865,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3880,13 +3880,13 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="G4:G7 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4123,7 +4123,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Chore: removed simulation_viz dependency on set_up_grasp_models
simulation_viz used thermodynamics_checks from set_up_grasp_models
which have now been copied over, so that the user doesn't
need to install set_up_grasp_models and its annoying equilibrator-api
dependency.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">max (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_mean (mmol/L/h)</t>
   </si>
   <si>
     <t xml:space="preserve">vref_std (mmol/L/h)</t>
@@ -484,13 +487,13 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="G4:G7 B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
@@ -616,15 +619,15 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="G4:G7 C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
@@ -636,7 +639,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +727,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="G4:G7 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,16 +740,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +967,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="G4:G7 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -979,13 +982,13 @@
         <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,8 +1289,8 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4:G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1306,37 +1309,37 @@
         <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,13 +1347,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>23</v>
@@ -1367,16 +1370,16 @@
         <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1390,16 +1393,16 @@
         <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>26</v>
@@ -1416,13 +1419,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1436,13 +1439,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1456,16 +1459,16 @@
         <v>43</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1479,16 +1482,16 @@
         <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>26</v>
@@ -1505,7 +1508,7 @@
         <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1519,7 +1522,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1533,7 +1536,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1547,7 +1550,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1561,7 +1564,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1575,7 +1578,7 @@
         <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1589,7 +1592,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1617,7 +1620,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="G4:G7 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2619,7 +2622,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G4:G7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3070,14 +3073,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="G4:G7 E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
@@ -3320,7 +3323,7 @@
   <dimension ref="A2:A16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="1" sqref="G4:G7 F26"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3422,7 +3425,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="1" sqref="G4:G7 G21"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3554,7 +3557,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="G4:G7 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3686,14 +3689,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="G4:G7 C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
@@ -3881,7 +3884,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="G4:G7 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Chore: instead of checking thermodynamics, only return dG+fluxes
On simulation_viz, visualize_MCA.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -492,8 +492,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
@@ -620,7 +620,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -650,7 +650,8 @@
         <v>-22.0149320730417</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.10350536706976</v>
+        <f aca="false">ABS(0.1*B2)</f>
+        <v>2.20149320730417</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +662,8 @@
         <v>0.285369137837419</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
+        <f aca="false">ABS(0.1*B3)</f>
+        <v>0.0285369137837419</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,7 +674,8 @@
         <v>0.0578197638950879</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
+        <f aca="false">ABS(0.1*B4)</f>
+        <v>0.00578197638950879</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,7 +686,8 @@
         <v>-0.00439408376660814</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
+        <f aca="false">ABS(0.1*B5)</f>
+        <v>0.000439408376660814</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +698,8 @@
         <v>6.84865633256387</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
+        <f aca="false">ABS(0.1*B6)</f>
+        <v>0.684865633256387</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,7 +710,8 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">ABS(0.1*B7)</f>
+        <v>0.000242684925806694</v>
       </c>
     </row>
   </sheetData>
@@ -3696,7 +3702,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Tests: updated unit tests after adding linprog support
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="106">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">FMINCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP solver (linprog or gurobi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gurobi</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
@@ -484,15 +490,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
@@ -531,58 +537,58 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -590,14 +596,22 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -619,7 +633,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -633,18 +647,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-22.0149320730417</v>
@@ -656,7 +670,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.285369137837419</v>
@@ -668,7 +682,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0578197638950879</v>
@@ -680,7 +694,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.00439408376660814</v>
@@ -692,7 +706,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.84865633256387</v>
@@ -704,7 +718,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.00242684925806694</v>
@@ -746,21 +760,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938745891927311</v>
@@ -774,7 +788,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.918129270809538</v>
@@ -788,7 +802,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.979330692978098</v>
@@ -802,7 +816,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.870960152966783</v>
@@ -816,7 +830,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.8</v>
@@ -830,7 +844,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -844,7 +858,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -858,7 +872,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -872,7 +886,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -886,7 +900,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -900,7 +914,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -914,7 +928,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -928,7 +942,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -942,7 +956,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -985,21 +999,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.729362608113343</v>
@@ -1013,7 +1027,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -1027,7 +1041,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -1041,7 +1055,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -1055,7 +1069,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1069,7 +1083,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.985171462369796</v>
@@ -1083,7 +1097,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.875198318353468</v>
@@ -1097,7 +1111,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.992232956019871</v>
@@ -1111,7 +1125,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.87219768970854</v>
@@ -1125,7 +1139,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.997064475108798</v>
@@ -1139,7 +1153,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1153,7 +1167,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.935839477601494</v>
@@ -1167,7 +1181,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1181,7 +1195,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1195,7 +1209,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.864112211147392</v>
@@ -1209,7 +1223,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1223,7 +1237,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1237,7 +1251,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.980827889050257</v>
@@ -1251,7 +1265,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.983205843276524</v>
@@ -1265,7 +1279,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.986809036820528</v>
@@ -1312,57 +1326,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1373,19 +1387,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1396,22 +1410,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1422,16 +1436,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1442,16 +1456,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1462,19 +1476,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1485,22 +1499,22 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1511,10 +1525,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1525,10 +1539,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1539,10 +1553,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1553,10 +1567,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1567,10 +1581,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1581,10 +1595,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1595,10 +1609,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1636,72 +1650,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1766,7 +1780,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1831,7 +1845,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1896,7 +1910,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1961,7 +1975,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2026,7 +2040,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2091,7 +2105,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-1</v>
@@ -2156,7 +2170,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2221,7 +2235,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2286,7 +2300,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2351,7 +2365,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2416,7 +2430,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2481,7 +2495,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2546,7 +2560,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2642,30 +2656,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2682,10 +2696,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2702,10 +2716,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2722,10 +2736,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2742,10 +2756,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2762,10 +2776,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2782,10 +2796,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2802,10 +2816,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2822,10 +2836,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2842,10 +2856,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2862,10 +2876,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2882,10 +2896,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2902,10 +2916,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2922,10 +2936,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2942,10 +2956,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2962,10 +2976,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2982,10 +2996,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -3002,10 +3016,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -3022,10 +3036,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -3042,10 +3056,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -3093,27 +3107,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -3124,10 +3138,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -3138,10 +3152,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -3152,10 +3166,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -3164,15 +3178,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -3181,15 +3195,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -3200,10 +3214,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -3214,10 +3228,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -3228,10 +3242,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3242,10 +3256,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3256,10 +3270,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -3270,10 +3284,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -3284,10 +3298,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -3298,10 +3312,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -3339,77 +3353,77 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3441,107 +3455,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3573,107 +3587,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3708,18 +3722,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3730,7 +3744,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3741,7 +3755,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3752,7 +3766,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3763,7 +3777,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-23.24</v>
@@ -3774,7 +3788,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-43.2</v>
@@ -3785,7 +3799,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-24.6</v>
@@ -3796,7 +3810,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-40</v>
@@ -3807,7 +3821,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-10</v>
@@ -3818,7 +3832,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-30</v>
@@ -3829,7 +3843,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3840,7 +3854,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3851,7 +3865,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3862,7 +3876,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>-10</v>
@@ -3900,18 +3914,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.65155467201437E-005</v>
@@ -3922,7 +3936,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3933,7 +3947,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3944,7 +3958,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3955,7 +3969,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3966,7 +3980,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00161010544336061</v>
@@ -3977,7 +3991,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.0018583615823201</v>
@@ -3988,7 +4002,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00102168275785283</v>
@@ -3999,7 +4013,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0171065051554435</v>
@@ -4010,7 +4024,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00285146987847134</v>
@@ -4021,7 +4035,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1E-012</v>
@@ -4032,7 +4046,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0013710175574537</v>
@@ -4043,7 +4057,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -4054,7 +4068,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -4065,7 +4079,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.37459615540709E-005</v>
@@ -4076,7 +4090,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -4087,7 +4101,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1E-012</v>
@@ -4098,7 +4112,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6.69219105835325E-006</v>
@@ -4109,7 +4123,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.00351539405111918</v>
@@ -4120,7 +4134,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.000588959799304437</v>

</xml_diff>

<commit_message>
chore: Set sampling mode to only GRASP or rejection
Previously we used the name ORACLE instead of GRASP
and also had other samplers that were actually not
supported, these have been removed.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -43,13 +43,13 @@
     <t xml:space="preserve">toy_model</t>
   </si>
   <si>
-    <t xml:space="preserve">Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORACLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLP solver (NLOPT, OPTI, FMINCON (default))</t>
+    <t xml:space="preserve">Sampling mode (GRASP or rejection)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRASP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP solver (NLOPT or FMINCON (default))</t>
   </si>
   <si>
     <t xml:space="preserve">FMINCON</t>
@@ -493,12 +493,12 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>

</xml_diff>

<commit_message>
Chore: Remove Percentile of alive models for SMC
Removed that line from general sheet on
excel file, since it is not used anywhere.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="105">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentile of alive models for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
   </si>
   <si>
     <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
@@ -490,10 +487,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -585,6 +582,9 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -598,23 +598,16 @@
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -647,18 +640,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-22.0149320730417</v>
@@ -670,7 +663,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.285369137837419</v>
@@ -682,7 +675,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0578197638950879</v>
@@ -694,7 +687,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.00439408376660814</v>
@@ -706,7 +699,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.84865633256387</v>
@@ -718,7 +711,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.00242684925806694</v>
@@ -760,21 +753,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938745891927311</v>
@@ -788,7 +781,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.918129270809538</v>
@@ -802,7 +795,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.979330692978098</v>
@@ -816,7 +809,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.870960152966783</v>
@@ -830,7 +823,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.8</v>
@@ -844,7 +837,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -858,7 +851,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -872,7 +865,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -886,7 +879,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -900,7 +893,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -914,7 +907,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -928,7 +921,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -942,7 +935,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -956,7 +949,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -999,21 +992,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.729362608113343</v>
@@ -1027,7 +1020,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -1041,7 +1034,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -1055,7 +1048,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -1069,7 +1062,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1083,7 +1076,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.985171462369796</v>
@@ -1097,7 +1090,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.875198318353468</v>
@@ -1111,7 +1104,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.992232956019871</v>
@@ -1125,7 +1118,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.87219768970854</v>
@@ -1139,7 +1132,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.997064475108798</v>
@@ -1153,7 +1146,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1167,7 +1160,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.935839477601494</v>
@@ -1181,7 +1174,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1195,7 +1188,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1209,7 +1202,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.864112211147392</v>
@@ -1223,7 +1216,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1237,7 +1230,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1251,7 +1244,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.980827889050257</v>
@@ -1265,7 +1258,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.983205843276524</v>
@@ -1279,7 +1272,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.986809036820528</v>
@@ -1326,57 +1319,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1387,19 +1380,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1410,22 +1403,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1436,16 +1429,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1456,16 +1449,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1476,19 +1469,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1499,22 +1492,22 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1525,10 +1518,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1539,10 +1532,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1553,10 +1546,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1567,10 +1560,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1581,10 +1574,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1595,10 +1588,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1609,10 +1602,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1650,72 +1643,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1780,7 +1773,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1845,7 +1838,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1910,7 +1903,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1975,7 +1968,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2040,7 +2033,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2105,7 +2098,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-1</v>
@@ -2170,7 +2163,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2235,7 +2228,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2300,7 +2293,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2365,7 +2358,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2430,7 +2423,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2495,7 +2488,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2560,7 +2553,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2656,30 +2649,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2696,10 +2689,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2716,10 +2709,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2736,10 +2729,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2756,10 +2749,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2776,10 +2769,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2796,10 +2789,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2816,10 +2809,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2836,10 +2829,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2856,10 +2849,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2876,10 +2869,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2896,10 +2889,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2916,10 +2909,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2936,10 +2929,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2956,10 +2949,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2976,10 +2969,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2996,10 +2989,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -3016,10 +3009,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -3036,10 +3029,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -3056,10 +3049,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -3107,27 +3100,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -3138,10 +3131,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -3152,10 +3145,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -3166,27 +3159,27 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -3195,15 +3188,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -3214,10 +3207,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -3228,10 +3221,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -3242,10 +3235,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3256,10 +3249,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3270,10 +3263,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -3284,10 +3277,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -3298,10 +3291,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -3312,10 +3305,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -3353,77 +3346,77 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3455,107 +3448,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3587,107 +3580,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3722,18 +3715,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3744,7 +3737,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3755,7 +3748,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3766,7 +3759,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3777,7 +3770,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-23.24</v>
@@ -3788,7 +3781,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-43.2</v>
@@ -3799,7 +3792,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-24.6</v>
@@ -3810,7 +3803,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-40</v>
@@ -3821,7 +3814,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-10</v>
@@ -3832,7 +3825,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-30</v>
@@ -3843,7 +3836,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3854,7 +3847,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3865,7 +3858,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3876,7 +3869,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>-10</v>
@@ -3914,18 +3907,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.65155467201437E-005</v>
@@ -3936,7 +3929,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3947,7 +3940,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3958,7 +3951,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3969,7 +3962,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3980,7 +3973,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00161010544336061</v>
@@ -3991,7 +3984,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.0018583615823201</v>
@@ -4002,7 +3995,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00102168275785283</v>
@@ -4013,7 +4006,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0171065051554435</v>
@@ -4024,7 +4017,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00285146987847134</v>
@@ -4035,7 +4028,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1E-012</v>
@@ -4046,7 +4039,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0013710175574537</v>
@@ -4057,7 +4050,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -4068,7 +4061,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -4079,7 +4072,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.37459615540709E-005</v>
@@ -4090,7 +4083,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -4101,7 +4094,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1E-012</v>
@@ -4112,7 +4105,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6.69219105835325E-006</v>
@@ -4123,7 +4116,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.00351539405111918</v>
@@ -4134,7 +4127,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.000588959799304437</v>

</xml_diff>

<commit_message>
Chore: Remove compute thermo from general sheet
Thermodynamics are computed by default, it's not
an option anymore.
The reason is that this is the most common use case
and it doesn't pay off to support the case where the
user provides the reaction dGs directly.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compute thermodynamics (ON = 1; OFF = 0)</t>
   </si>
   <si>
     <t xml:space="preserve">Initial tolerance (OPTIONAL)</t>
@@ -490,7 +487,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -590,23 +587,16 @@
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -640,18 +630,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-22.0149320730417</v>
@@ -663,7 +653,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.285369137837419</v>
@@ -675,7 +665,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0578197638950879</v>
@@ -687,7 +677,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.00439408376660814</v>
@@ -699,7 +689,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.84865633256387</v>
@@ -711,7 +701,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.00242684925806694</v>
@@ -753,21 +743,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938745891927311</v>
@@ -781,7 +771,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.918129270809538</v>
@@ -795,7 +785,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.979330692978098</v>
@@ -809,7 +799,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.870960152966783</v>
@@ -823,7 +813,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.8</v>
@@ -837,7 +827,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -851,7 +841,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -865,7 +855,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -879,7 +869,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -893,7 +883,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -907,7 +897,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -921,7 +911,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -935,7 +925,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -949,7 +939,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -992,21 +982,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.729362608113343</v>
@@ -1020,7 +1010,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -1034,7 +1024,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -1048,7 +1038,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -1062,7 +1052,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1076,7 +1066,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.985171462369796</v>
@@ -1090,7 +1080,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.875198318353468</v>
@@ -1104,7 +1094,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.992232956019871</v>
@@ -1118,7 +1108,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.87219768970854</v>
@@ -1132,7 +1122,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.997064475108798</v>
@@ -1146,7 +1136,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1160,7 +1150,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.935839477601494</v>
@@ -1174,7 +1164,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1188,7 +1178,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1202,7 +1192,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.864112211147392</v>
@@ -1216,7 +1206,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1230,7 +1220,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1244,7 +1234,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.980827889050257</v>
@@ -1258,7 +1248,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.983205843276524</v>
@@ -1272,7 +1262,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.986809036820528</v>
@@ -1319,57 +1309,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1380,19 +1370,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1403,22 +1393,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1429,16 +1419,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1449,16 +1439,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1469,19 +1459,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1492,22 +1482,22 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1518,10 +1508,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1532,10 +1522,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1546,10 +1536,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1560,10 +1550,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1574,10 +1564,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1588,10 +1578,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1602,10 +1592,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1643,72 +1633,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1773,7 +1763,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1838,7 +1828,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1903,7 +1893,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1968,7 +1958,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2033,7 +2023,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2098,7 +2088,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-1</v>
@@ -2163,7 +2153,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2228,7 +2218,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2293,7 +2283,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2358,7 +2348,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2423,7 +2413,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2488,7 +2478,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2553,7 +2543,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2649,30 +2639,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2689,10 +2679,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2709,10 +2699,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2729,10 +2719,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2749,10 +2739,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2769,10 +2759,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2789,10 +2779,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2809,10 +2799,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2829,10 +2819,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2849,10 +2839,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2869,10 +2859,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2889,10 +2879,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2909,10 +2899,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2929,10 +2919,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2949,10 +2939,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2969,10 +2959,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2989,10 +2979,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -3009,10 +2999,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -3029,10 +3019,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -3049,10 +3039,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -3100,27 +3090,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -3131,10 +3121,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -3145,10 +3135,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -3159,27 +3149,27 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -3188,15 +3178,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -3207,10 +3197,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -3221,10 +3211,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -3235,10 +3225,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3249,10 +3239,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3263,10 +3253,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -3277,10 +3267,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -3291,10 +3281,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -3305,10 +3295,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -3346,77 +3336,77 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3448,107 +3438,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3580,107 +3570,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3715,18 +3705,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3737,7 +3727,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3748,7 +3738,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3759,7 +3749,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3770,7 +3760,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-23.24</v>
@@ -3781,7 +3771,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-43.2</v>
@@ -3792,7 +3782,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-24.6</v>
@@ -3803,7 +3793,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-40</v>
@@ -3814,7 +3804,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-10</v>
@@ -3825,7 +3815,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-30</v>
@@ -3836,7 +3826,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3847,7 +3837,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3858,7 +3848,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3869,7 +3859,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>-10</v>
@@ -3907,18 +3897,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.65155467201437E-005</v>
@@ -3929,7 +3919,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3940,7 +3930,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3951,7 +3941,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3962,7 +3952,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3973,7 +3963,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00161010544336061</v>
@@ -3984,7 +3974,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.0018583615823201</v>
@@ -3995,7 +3985,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00102168275785283</v>
@@ -4006,7 +3996,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0171065051554435</v>
@@ -4017,7 +4007,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00285146987847134</v>
@@ -4028,7 +4018,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1E-012</v>
@@ -4039,7 +4029,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0013710175574537</v>
@@ -4050,7 +4040,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -4061,7 +4051,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -4072,7 +4062,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.37459615540709E-005</v>
@@ -4083,7 +4073,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -4094,7 +4084,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1E-012</v>
@@ -4105,7 +4095,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6.69219105835325E-006</v>
@@ -4116,7 +4106,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.00351539405111918</v>
@@ -4127,7 +4117,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.000588959799304437</v>

</xml_diff>

<commit_message>
Chore: Remove initial tolerance.
This was only used with the SMC samplers, which
are no longer supported.
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="103">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -79,10 +79,7 @@
     <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">Initial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final tolerance (in the case of ORACLE, set to 1)</t>
+    <t xml:space="preserve">Final tolerance (in the case of GRASP, set to 1)</t>
   </si>
   <si>
     <t xml:space="preserve">rxn ID</t>
@@ -487,7 +484,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,15 +584,11 @@
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -630,18 +623,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-22.0149320730417</v>
@@ -653,7 +646,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.285369137837419</v>
@@ -665,7 +658,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.0578197638950879</v>
@@ -677,7 +670,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.00439408376660814</v>
@@ -689,7 +682,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.84865633256387</v>
@@ -701,7 +694,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.00242684925806694</v>
@@ -743,21 +736,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938745891927311</v>
@@ -771,7 +764,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.918129270809538</v>
@@ -785,7 +778,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.979330692978098</v>
@@ -799,7 +792,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.870960152966783</v>
@@ -813,7 +806,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.8</v>
@@ -827,7 +820,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -841,7 +834,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -855,7 +848,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -869,7 +862,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -883,7 +876,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -897,7 +890,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -911,7 +904,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -925,7 +918,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -939,7 +932,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -982,21 +975,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.729362608113343</v>
@@ -1010,7 +1003,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -1024,7 +1017,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -1038,7 +1031,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -1052,7 +1045,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1066,7 +1059,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.985171462369796</v>
@@ -1080,7 +1073,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.875198318353468</v>
@@ -1094,7 +1087,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.992232956019871</v>
@@ -1108,7 +1101,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.87219768970854</v>
@@ -1122,7 +1115,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.997064475108798</v>
@@ -1136,7 +1129,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -1150,7 +1143,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.935839477601494</v>
@@ -1164,7 +1157,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1178,7 +1171,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1192,7 +1185,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.864112211147392</v>
@@ -1206,7 +1199,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1220,7 +1213,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1234,7 +1227,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.980827889050257</v>
@@ -1248,7 +1241,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.983205843276524</v>
@@ -1262,7 +1255,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.986809036820528</v>
@@ -1309,57 +1302,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1370,19 +1363,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1393,22 +1386,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1419,16 +1412,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1439,16 +1432,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1459,19 +1452,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1482,22 +1475,22 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1508,10 +1501,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1522,10 +1515,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1536,10 +1529,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1550,10 +1543,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1564,10 +1557,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1578,10 +1571,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1592,10 +1585,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1633,72 +1626,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1763,7 +1756,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1828,7 +1821,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1893,7 +1886,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1958,7 +1951,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2023,7 +2016,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2088,7 +2081,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-1</v>
@@ -2153,7 +2146,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2218,7 +2211,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2283,7 +2276,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2348,7 +2341,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2413,7 +2406,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2478,7 +2471,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2543,7 +2536,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2639,30 +2632,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2679,10 +2672,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2699,10 +2692,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2719,10 +2712,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2739,10 +2732,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2759,10 +2752,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2779,10 +2772,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2799,10 +2792,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2819,10 +2812,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2839,10 +2832,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2859,10 +2852,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2879,10 +2872,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2899,10 +2892,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2919,10 +2912,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2939,10 +2932,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2959,10 +2952,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2979,10 +2972,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -2999,10 +2992,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -3019,10 +3012,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -3039,10 +3032,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -3090,27 +3083,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -3121,10 +3114,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -3135,10 +3128,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -3149,27 +3142,27 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -3178,15 +3171,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -3197,10 +3190,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -3211,10 +3204,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -3225,10 +3218,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -3239,10 +3232,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3253,10 +3246,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -3267,10 +3260,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -3281,10 +3274,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -3295,10 +3288,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -3336,77 +3329,77 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3438,107 +3431,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3570,107 +3563,107 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3705,18 +3698,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3727,7 +3720,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3738,7 +3731,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3749,7 +3742,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3760,7 +3753,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-23.24</v>
@@ -3771,7 +3764,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-43.2</v>
@@ -3782,7 +3775,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-24.6</v>
@@ -3793,7 +3786,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-40</v>
@@ -3804,7 +3797,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-10</v>
@@ -3815,7 +3808,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-30</v>
@@ -3826,7 +3819,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3837,7 +3830,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3848,7 +3841,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3859,7 +3852,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>-10</v>
@@ -3897,18 +3890,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.65155467201437E-005</v>
@@ -3919,7 +3912,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3930,7 +3923,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3941,7 +3934,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3952,7 +3945,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3963,7 +3956,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00161010544336061</v>
@@ -3974,7 +3967,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.0018583615823201</v>
@@ -3985,7 +3978,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00102168275785283</v>
@@ -3996,7 +3989,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0171065051554435</v>
@@ -4007,7 +4000,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00285146987847134</v>
@@ -4018,7 +4011,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1E-012</v>
@@ -4029,7 +4022,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.0013710175574537</v>
@@ -4040,7 +4033,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -4051,7 +4044,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -4062,7 +4055,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.37459615540709E-005</v>
@@ -4073,7 +4066,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -4084,7 +4077,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1E-012</v>
@@ -4095,7 +4088,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>6.69219105835325E-006</v>
@@ -4106,7 +4099,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.00351539405111918</v>
@@ -4117,7 +4110,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.000588959799304437</v>

</xml_diff>

<commit_message>
Chore: Updated mets and rxns sheets in excel files
</commit_message>
<xml_diff>
--- a/io/input/toy_model.xlsx
+++ b/io/input/toy_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="100">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -196,12 +196,6 @@
     <t xml:space="preserve">balanced?</t>
   </si>
   <si>
-    <t xml:space="preserve">active?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constant?</t>
-  </si>
-  <si>
     <t xml:space="preserve">measured?</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">transport reaction?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelled?</t>
   </si>
   <si>
     <t xml:space="preserve">isoenzymes</t>
@@ -483,13 +474,13 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
@@ -623,13 +614,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,16 +727,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,13 +969,13 @@
         <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,40 +1293,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,13 +1334,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>22</v>
@@ -1366,16 +1357,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1389,16 +1380,16 @@
         <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>25</v>
@@ -1415,13 +1406,13 @@
         <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1435,13 +1426,13 @@
         <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1455,16 +1446,16 @@
         <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1478,16 +1469,16 @@
         <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>25</v>
@@ -1504,7 +1495,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1518,7 +1509,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1532,7 +1523,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1546,7 +1537,7 @@
         <v>47</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1560,7 +1551,7 @@
         <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1574,7 +1565,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1588,7 +1579,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -2615,19 +2606,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,14 +2630,8 @@
       <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,12 +2647,6 @@
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -2681,12 +2659,6 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2701,12 +2673,6 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2721,12 +2687,6 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2743,12 +2703,6 @@
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -2763,12 +2717,6 @@
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -2783,12 +2731,6 @@
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
@@ -2803,12 +2745,6 @@
       <c r="D9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
@@ -2823,12 +2759,6 @@
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
@@ -2843,12 +2773,6 @@
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
@@ -2863,12 +2787,6 @@
       <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -2883,12 +2801,6 @@
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
@@ -2903,12 +2815,6 @@
       <c r="D14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
@@ -2923,12 +2829,6 @@
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
@@ -2943,12 +2843,6 @@
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
@@ -2961,12 +2855,6 @@
         <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2981,12 +2869,6 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3003,12 +2885,6 @@
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
@@ -3023,12 +2899,6 @@
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
@@ -3041,12 +2911,6 @@
         <v>0</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3066,36 +2930,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,9 +2969,6 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -3122,9 +2980,6 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -3136,25 +2991,19 @@
       <c r="C4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>63</v>
+      <c r="D5" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,16 +3011,13 @@
         <v>41</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>63</v>
+      <c r="D6" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3184,9 +3030,6 @@
       <c r="C7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -3198,9 +3041,6 @@
       <c r="C8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
@@ -3212,9 +3052,6 @@
       <c r="C9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
@@ -3226,9 +3063,6 @@
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
@@ -3240,9 +3074,6 @@
       <c r="C11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
@@ -3254,9 +3085,6 @@
       <c r="C12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -3268,9 +3096,6 @@
       <c r="C13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
@@ -3282,9 +3107,6 @@
       <c r="C14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
@@ -3295,9 +3117,6 @@
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3329,7 +3148,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3698,13 +3517,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,10 +3712,10 @@
         <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>